<commit_message>
Use short xlsx sheet names
Define short sheet names in
01-generate-pedot-column-display-order-name-xlsx.py.

Renamed utils.TSV class to utils.TSVSheet class. Initialize
utils.TSVSheet class with sheet name and TSV path.
</commit_message>
<xml_diff>
--- a/analyses/pedot-table-column-display-order-name/results/pedot-table-column-display-order-name.xlsx
+++ b/analyses/pedot-table-column-display-order-name/results/pedot-table-column-display-order-name.xlsx
@@ -4,16 +4,16 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="gene-level-snv-consensus-annotated-mut-freq.jsonl.gz" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="variant-level-snv-consensus-annotated-mut-freq.jsonl.gz" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="gene-level-cnv-consensus-annotated-mut-freq.jsonl.gz" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="putative-oncogene-fused-gene-freq.jsonl.gz" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="putative-oncogene-fusion-freq.jsonl.gz" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="long_n_tpm_mean_sd_quantile_gene_wise_zscore.jsonl.gz" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="long_n_tpm_mean_sd_quantile_group_wise_zscore.jsonl.gz" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="SNV gene-level" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="SNV variant-level" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="CNV gene-level" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Fusion gene-level" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Fusion fusion-level" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="TPM stats gene-wise z-scores" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="TPM stats group-wise z-scores" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -50,83 +50,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -422,10 +354,10 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane activePane="bottomRight" state="frozen" topLeftCell="C2" xSplit="2" ySplit="1"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1651,7 +1583,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -1664,10 +1596,10 @@
   <dimension ref="A1:AC12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane activePane="bottomRight" state="frozen" topLeftCell="C2" xSplit="2" ySplit="1"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -3293,7 +3225,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -3306,10 +3238,10 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane activePane="bottomRight" state="frozen" topLeftCell="C2" xSplit="2" ySplit="1"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -4355,7 +4287,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -4368,10 +4300,10 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane activePane="bottomRight" state="frozen" topLeftCell="C2" xSplit="2" ySplit="1"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -5233,7 +5165,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -5246,10 +5178,10 @@
   <dimension ref="A1:AB12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane activePane="bottomRight" state="frozen" topLeftCell="C2" xSplit="2" ySplit="1"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -6667,7 +6599,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -6680,10 +6612,10 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane activePane="bottomRight" state="frozen" topLeftCell="C2" xSplit="2" ySplit="1"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -7489,7 +7421,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -7502,10 +7434,10 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane activePane="bottomRight" state="frozen" topLeftCell="C2" xSplit="2" ySplit="1"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" pane="bottomRight" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -8311,6 +8243,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add column name and order changes for PedOT display
Replace RMTL with PMTL.

Move Variant_ID_hg38 and Protein_change columns after the Gene_symbol
column.
</commit_message>
<xml_diff>
--- a/analyses/pedot-table-column-display-order-name/results/pedot-table-column-display-order-name.xlsx
+++ b/analyses/pedot-table-column-display-order-name/results/pedot-table-column-display-order-name.xlsx
@@ -380,7 +380,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>RMTL</t>
+          <t>PMTL</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -1622,87 +1622,87 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>RMTL</t>
+          <t>Variant ID hg38</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>Protein change</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>PMTL</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>Dataset</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Disease</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>EFO</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>MONDO</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Variant ID hg38</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>dbSNP ID</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>VEP impact</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>SIFT impact</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>PolyPhen impact</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>Variant classification</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>Variant type</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>Gene full name</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>Protein RefSeq ID</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>Gene Ensembl ID</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>Protein Ensembl ID</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>Protein change</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
@@ -1767,85 +1767,85 @@
           <t>HEXA</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>chr15_72349245_G_T</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>p.L285M</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>TARGET</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Neuroblastoma</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>EFO_0000621</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>MONDO_0005072</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>chr15_72349245_G_T</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>novel</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>MODERATE</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>deleterious(0)</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>probably_damaging(0.985)</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>Missense_Mutation</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>SNP</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>hexosaminidase subunit alpha</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>NP_000511.2,NP_001305754.1</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>ENSG00000213614</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>ENSP00000455114</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>p.L285M</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -1902,85 +1902,85 @@
           <t>WNT4</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>chr1_22129778_G_T</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>p.Q51K</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>TARGET</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Neuroblastoma</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>EFO_0000621</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>MONDO_0005072</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>chr1_22129778_G_T</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>novel</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>MODERATE</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>tolerated(0.92)</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>benign(0.003)</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>Missense_Mutation</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>SNP</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>Wnt family member 4</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>NP_110388.2</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>ENSG00000162552</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>ENSP00000290167</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>p.Q51K</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -2037,85 +2037,85 @@
           <t>PRPSAP1</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>chr17_76344671_C_A</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>p.R97I</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>TARGET</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Neuroblastoma</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>EFO_0000621</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>MONDO_0005072</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>chr17_76344671_C_A</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>novel</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>MODERATE</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>tolerated(0.09)</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>possibly_damaging(0.708)</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>Missense_Mutation</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>SNP</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>phosphoribosyl pyrophosphate synthetase associated protein 1</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="R4" t="inlineStr">
         <is>
           <t>NP_001317432.1,NP_001353165.1,NP_002757.2</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>ENSG00000161542</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>ENSP00000414624</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>p.R97I</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -2172,85 +2172,85 @@
           <t>ZNF334</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>chr20_46502227_T_C</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t>p.H371R</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>PBTA</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>Ependymoma</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>EFO_1000028</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>MONDO_0016698</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>chr20_46502227_T_C</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>novel</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>MODERATE</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>deleterious(0)</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>probably_damaging(0.986)</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>Missense_Mutation</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>SNP</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>zinc finger protein 334</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="R5" t="inlineStr">
         <is>
           <t>NP_001257426.1,NP_001340742.1,NP_001340743.1,NP_001340744.1,NP_001340745.1,NP_001340746.1,NP_001340747.1,NP_001340748.1,NP_001340749.1,NP_001340750.1,NP_001340751.1,NP_001340752.1,NP_001340753.1,NP_001340754.1,NP_001340755.1,NP_060572.3,NP_955473.1</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>ENSG00000198185</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>ENSP00000255129</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>p.H371R</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
@@ -2311,81 +2311,81 @@
           <t>MT-ND4</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>chrM_10922_A_G</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>p.T55A</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>PBTA</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Schwannoma</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>EFO_0000693</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>MONDO_0002546</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>chrM_10922_A_G</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>novel</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>MODERATE</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>tolerated_low_confidence(0.33)</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>benign(0.007)</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>Missense_Mutation</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>SNP</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>NADH dehydrogenase subunit 4</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr">
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr">
         <is>
           <t>ENSG00000198886</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
+      <c r="T6" t="inlineStr">
         <is>
           <t>ENSP00000354961</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>p.T55A</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
@@ -2442,77 +2442,77 @@
           <t>DNAI1</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>chr9_34506692_G_T</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>p.E381*</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>TARGET</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>Neuroblastoma</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>EFO_0000621</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>MONDO_0005072</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>chr9_34506692_G_T</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>novel</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr">
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
         <is>
           <t>Nonsense_Mutation</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>SNP</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>dynein axonemal intermediate chain 1</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
+      <c r="R7" t="inlineStr">
         <is>
           <t>NP_001268357.1,NP_036276.1</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr">
+      <c r="S7" t="inlineStr">
         <is>
           <t>ENSG00000122735</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
+      <c r="T7" t="inlineStr">
         <is>
           <t>ENSP00000480538</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>p.E381*</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
@@ -2565,85 +2565,85 @@
           <t>ZNF143</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>chr11_9512537_G_T</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
+          <t>p.V489L</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>PBTA</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>High-grade glioma/astrocytoma</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>EFO_0005543</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>MONDO_0100342</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>chr11_9512537_G_T</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>novel</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>MODERATE</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>tolerated(0.31)</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>possibly_damaging(0.785)</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>Missense_Mutation</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>SNP</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="Q8" t="inlineStr">
         <is>
           <t>zinc finger protein 143</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
+      <c r="R8" t="inlineStr">
         <is>
           <t>NP_001269585.1,NP_001269586.1,NP_003433.3</t>
         </is>
       </c>
-      <c r="R8" t="inlineStr">
+      <c r="S8" t="inlineStr">
         <is>
           <t>ENSG00000166478</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr">
+      <c r="T8" t="inlineStr">
         <is>
           <t>ENSP00000379847</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>p.V489L</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -2700,85 +2700,85 @@
           <t>ZFAND4</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>chr10_45626424_G_T</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
+          <t>p.H467N</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>all_cohorts</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>Neuroblastoma</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>EFO_0000621</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>MONDO_0005072</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>chr10_45626424_G_T</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>novel</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>MODERATE</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>tolerated(0.11)</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>benign(0.115)</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>Missense_Mutation</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>SNP</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>zinc finger AN1-type containing 4</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
+      <c r="R9" t="inlineStr">
         <is>
           <t>NP_001121796.1,NP_001269834.1,NP_001269835.1,NP_777550.2</t>
         </is>
       </c>
-      <c r="R9" t="inlineStr">
+      <c r="S9" t="inlineStr">
         <is>
           <t>ENSG00000172671</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr">
+      <c r="T9" t="inlineStr">
         <is>
           <t>ENSP00000339484</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>p.H467N</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
@@ -2831,85 +2831,85 @@
           <t>OR2C1</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>chr16_3355948_G_T</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>p.G3V</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>all_cohorts</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>Neuroblastoma</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>EFO_0000621</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>MONDO_0005072</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>chr16_3355948_G_T</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>novel</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>MODERATE</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>tolerated(0.28)</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>benign(0)</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>Missense_Mutation</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>SNP</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>olfactory receptor family 2 subfamily C member 1</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="R10" t="inlineStr">
         <is>
           <t>NP_036500.2</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr">
+      <c r="S10" t="inlineStr">
         <is>
           <t>ENSG00000168158</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr">
+      <c r="T10" t="inlineStr">
         <is>
           <t>ENSP00000307726</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>p.G3V</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -2962,85 +2962,85 @@
           <t>RBM5</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>chr3_50109641_C_A</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr">
         <is>
+          <t>p.Q411K</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>TARGET</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>Neuroblastoma</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>EFO_0000621</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>MONDO_0005072</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>chr3_50109641_C_A</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>novel</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>MODERATE</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>tolerated(0.09)</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>possibly_damaging(0.678)</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>Missense_Mutation</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>SNP</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>RNA binding motif protein 5</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr">
+      <c r="R11" t="inlineStr">
         <is>
           <t>NP_005769.1</t>
         </is>
       </c>
-      <c r="R11" t="inlineStr">
+      <c r="S11" t="inlineStr">
         <is>
           <t>ENSG00000003756</t>
         </is>
       </c>
-      <c r="S11" t="inlineStr">
+      <c r="T11" t="inlineStr">
         <is>
           <t>ENSP00000343054</t>
-        </is>
-      </c>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>p.Q411K</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
@@ -3095,87 +3095,87 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
+          <t>Variant_ID_hg38</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Protein_change</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
           <t>RMTL</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>Dataset</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>Disease</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>EFO</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>MONDO</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Variant_ID_hg38</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>dbSNP_ID</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t>VEP_impact</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="M12" t="inlineStr">
         <is>
           <t>SIFT_impact</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="N12" t="inlineStr">
         <is>
           <t>PolyPhen_impact</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="O12" t="inlineStr">
         <is>
           <t>Variant_classification</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>Variant_type</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>Gene_full_name</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="R12" t="inlineStr">
         <is>
           <t>Protein_RefSeq_ID</t>
         </is>
       </c>
-      <c r="R12" t="inlineStr">
+      <c r="S12" t="inlineStr">
         <is>
           <t>Gene_Ensembl_ID</t>
         </is>
       </c>
-      <c r="S12" t="inlineStr">
+      <c r="T12" t="inlineStr">
         <is>
           <t>Protein_Ensembl_ID</t>
-        </is>
-      </c>
-      <c r="T12" t="inlineStr">
-        <is>
-          <t>Protein_change</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
@@ -3324,7 +3324,7 @@
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>RMTL</t>
+          <t>PMTL</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
@@ -4341,7 +4341,7 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>RMTL</t>
+          <t>PMTL</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
@@ -5284,7 +5284,7 @@
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>RMTL</t>
+          <t>PMTL</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
@@ -6638,7 +6638,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>RMTL</t>
+          <t>PMTL</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -7460,7 +7460,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>RMTL</t>
+          <t>PMTL</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">

</xml_diff>

<commit_message>
Revise result xlsx file user guide
</commit_message>
<xml_diff>
--- a/analyses/pedot-table-column-display-order-name/results/pedot-table-column-display-order-name.xlsx
+++ b/analyses/pedot-table-column-display-order-name/results/pedot-table-column-display-order-name.xlsx
@@ -809,7 +809,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Please do not change the order or values of the first two columns.</t>
+          <t>Delete one or more columns to advise PedOT website not to display the deleted columns.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -926,7 +926,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Please do not change the values of the last row.</t>
+          <t>Please do not change the order or values of the first two columns.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1033,7 +1033,11 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Please do not delete the first or the second column.</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>Sample row #6</t>
@@ -1142,7 +1146,11 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Please do not change the values of the last row.</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>Sample row #7</t>
@@ -1251,7 +1259,11 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Please do not delete any row.</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>Sample row #8</t>
@@ -7213,7 +7225,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Please do not change the order or values of the first two columns.</t>
+          <t>Delete one or more columns to advise PedOT website not to display the deleted columns.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -7356,291 +7368,299 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Please do not change the order or values of the first two columns.</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Sample row #5</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>BRIP1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>chr17_61683414_C_T</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>p.G1211D</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Relevant Molecular Target (RMTL version 1.0)</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>PBTA</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>High-grade glioma/astrocytoma</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>EFO_0005543</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>MONDO_0100342</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>novel</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>MODERATE</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>tolerated_low_confidence(1)</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>benign(0.009)</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Missense_Mutation</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>SNP</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>BRCA1 interacting helicase 1</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>NP_114432.2</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>ENSG00000136492</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>ENSP00000259008</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>1/50</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>2.00%</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>0/30</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>1/21</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>4.76%</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>TumorSuppressorGene</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Please do not delete the first or the second column.</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Sample row #6</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>PSMC5</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>chr17_63831748_T_C</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>p.Y369H</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Relevant Molecular Target (RMTL version 1.0)</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>PBTA</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>High-grade glioma/astrocytoma</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>EFO_0005543</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>MONDO_0100342</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>novel</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>MODERATE</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>deleterious(0)</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>possibly_damaging(0.497)</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Missense_Mutation</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>SNP</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>proteasome 26S subunit, ATPase 5</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>NP_001186092.1,NP_002796.4</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>ENSG00000087191</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>ENSP00000310572</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>1/50</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>2.00%</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>1/30</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>3.33%</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>0/21</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>0.00%</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>Please do not change the values of the last row.</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Sample row #5</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>BRIP1</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>chr17_61683414_C_T</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>p.G1211D</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Relevant Molecular Target (RMTL version 1.0)</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>PBTA</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>High-grade glioma/astrocytoma</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>EFO_0005543</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>MONDO_0100342</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>novel</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>MODERATE</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>tolerated_low_confidence(1)</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>benign(0.009)</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>Missense_Mutation</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>SNP</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>BRCA1 interacting helicase 1</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>NP_114432.2</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>ENSG00000136492</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>ENSP00000259008</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>1/50</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>2.00%</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>0/30</t>
-        </is>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>1/21</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>4.76%</t>
-        </is>
-      </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>TumorSuppressorGene</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Sample row #6</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>PSMC5</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>chr17_63831748_T_C</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>p.Y369H</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Relevant Molecular Target (RMTL version 1.0)</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>PBTA</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>High-grade glioma/astrocytoma</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>EFO_0005543</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>MONDO_0100342</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>novel</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>MODERATE</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>deleterious(0)</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>possibly_damaging(0.497)</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>Missense_Mutation</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>SNP</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>proteasome 26S subunit, ATPase 5</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>NP_001186092.1,NP_002796.4</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>ENSG00000087191</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>ENSP00000310572</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>1/50</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>2.00%</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>1/30</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>3.33%</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>0/21</t>
-        </is>
-      </c>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>0.00%</t>
-        </is>
-      </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="AC7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
           <t>Sample row #7</t>
@@ -7775,7 +7795,11 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Please do not delete any row.</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>Sample row #8</t>
@@ -15417,7 +15441,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Please do not change the order or values of the first two columns.</t>
+          <t>Delete one or more columns to advise PedOT website not to display the deleted columns.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -15507,7 +15531,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Please do not change the values of the last row.</t>
+          <t>Please do not change the order or values of the first two columns.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -15595,7 +15619,11 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Please do not delete the first or the second column.</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>Sample row #6</t>
@@ -15681,7 +15709,11 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Please do not change the values of the last row.</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>Sample row #7</t>
@@ -15763,7 +15795,11 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Please do not delete any row.</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>Sample row #8</t>
@@ -20747,7 +20783,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Please do not change the order or values of the first two columns.</t>
+          <t>Delete one or more columns to advise PedOT website not to display the deleted columns.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -20824,7 +20860,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Please do not change the values of the last row.</t>
+          <t>Please do not change the order or values of the first two columns.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -20895,7 +20931,11 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Please do not delete the first or the second column.</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>Sample row #6</t>
@@ -20968,7 +21008,11 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Please do not change the values of the last row.</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>Sample row #7</t>
@@ -21037,7 +21081,11 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Please do not delete any row.</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>Sample row #8</t>
@@ -25383,7 +25431,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Please do not change the order or values of the first two columns.</t>
+          <t>Delete one or more columns to advise PedOT website not to display the deleted columns.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -25505,7 +25553,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Please do not change the values of the last row.</t>
+          <t>Please do not change the order or values of the first two columns.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -25625,7 +25673,11 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Please do not delete the first or the second column.</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>Sample row #6</t>
@@ -25743,7 +25795,11 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Please do not change the values of the last row.</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>Sample row #7</t>
@@ -25861,7 +25917,11 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Please do not delete any row.</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>Sample row #8</t>
@@ -32337,7 +32397,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Please do not change the order or values of the first two columns.</t>
+          <t>Delete one or more columns to advise PedOT website not to display the deleted columns.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -32405,7 +32465,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Please do not change the values of the last row.</t>
+          <t>Please do not change the order or values of the first two columns.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -32475,7 +32535,11 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Please do not delete the first or the second column.</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>Sample row #6</t>
@@ -32539,7 +32603,11 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Please do not change the values of the last row.</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>Sample row #7</t>
@@ -32603,7 +32671,11 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Please do not delete any row.</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>Sample row #8</t>
@@ -36523,7 +36595,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Please do not change the order or values of the first two columns.</t>
+          <t>Delete one or more columns to advise PedOT website not to display the deleted columns.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -36591,7 +36663,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Please do not change the values of the last row.</t>
+          <t>Please do not change the order or values of the first two columns.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -36661,7 +36733,11 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Please do not delete the first or the second column.</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>Sample row #6</t>
@@ -36725,7 +36801,11 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Please do not change the values of the last row.</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>Sample row #7</t>
@@ -36789,7 +36869,11 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Please do not delete any row.</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>Sample row #8</t>

</xml_diff>